<commit_message>
tiny change to excel input for cond 2
</commit_message>
<xml_diff>
--- a/excel_input_files/Test_input_Condition2Pos.xlsx
+++ b/excel_input_files/Test_input_Condition2Pos.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Glasgow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/git/lipid_prototype/excel_input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1667AC-7434-4B0A-A7D2-0DAF0C9023CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2A22EB-0BAE-E745-84BE-AB154EFA3431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="lipids" sheetId="3" r:id="rId1"/>
+    <sheet name="files" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>C42H82NO8P</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>pc 34:1</t>
   </si>
   <si>
-    <t>Formula</t>
-  </si>
-  <si>
     <t>ion</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t>files to exclude</t>
   </si>
   <si>
-    <t>Filename</t>
-  </si>
-  <si>
     <t>timepoint</t>
   </si>
   <si>
@@ -272,6 +263,15 @@
   </si>
   <si>
     <t>120_d20_pos_2</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>filename</t>
   </si>
 </sst>
 </file>
@@ -666,56 +666,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D248679-4876-F949-8D23-26F678A03F89}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>760.58360000000005</v>
@@ -730,15 +730,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>758.56769999999995</v>
@@ -753,18 +753,18 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>760.58408376174998</v>
@@ -779,15 +779,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>786.59949562139604</v>
@@ -802,15 +802,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>746.60507156904896</v>
@@ -825,15 +825,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>758.56817165437201</v>
@@ -852,15 +852,15 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>788.61553198915601</v>
@@ -875,15 +875,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>772.62058032957498</v>
@@ -898,15 +898,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>813.68350858249198</v>
@@ -921,15 +921,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>744.58931973768995</v>
@@ -944,15 +944,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>784.58390749345904</v>
@@ -967,15 +967,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>876.79998613835096</v>
@@ -990,15 +990,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>850.78518979760804</v>
@@ -1013,15 +1013,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>774.59980867596096</v>
@@ -1036,15 +1036,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <v>814.63036786387795</v>
@@ -1059,15 +1059,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D17">
         <v>774.63657999677696</v>
@@ -1082,15 +1082,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>720.55305447337798</v>
@@ -1105,15 +1105,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <v>772.58393455538999</v>
@@ -1128,15 +1128,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>732.58963722401495</v>
@@ -1151,15 +1151,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
         <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
       </c>
       <c r="D21">
         <v>902.81555025753801</v>
@@ -1177,15 +1177,15 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D22">
         <v>730.53751278662298</v>
@@ -1200,15 +1200,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D23">
         <v>744.55317308196697</v>
@@ -1223,15 +1223,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D24">
         <v>810.59602938915702</v>
@@ -1246,18 +1246,18 @@
         <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D25">
         <v>834.59924485985698</v>
@@ -1272,18 +1272,18 @@
         <v>10</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D26">
         <v>734.56838307922601</v>
@@ -1298,18 +1298,18 @@
         <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D27">
         <v>550.38647215227797</v>
@@ -1324,18 +1324,18 @@
         <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <v>480.30816700870099</v>
@@ -1350,18 +1350,18 @@
         <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D29">
         <v>502.29250656260803</v>
@@ -1376,18 +1376,18 @@
         <v>10</v>
       </c>
       <c r="H29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D30">
         <v>816.64664565839496</v>
@@ -1402,18 +1402,18 @@
         <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D31">
         <v>814.63036786387795</v>
@@ -1428,18 +1428,18 @@
         <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D32">
         <v>834.5992</v>
@@ -1454,18 +1454,18 @@
         <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D33">
         <v>794.60432067756005</v>
@@ -1480,7 +1480,7 @@
         <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1494,74 +1494,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D3203F-BC1B-7745-B9F8-C5C7D6E73FC7}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B4">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B8">
         <v>120</v>

</xml_diff>